<commit_message>
Adding WRLD to fixed COL elect
</commit_message>
<xml_diff>
--- a/data-raw/FixedCOLElect.xlsx
+++ b/data-raw/FixedCOLElect.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/IEATools/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AFB1AEA-F39F-7347-87D7-4D29CA01A3AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CFF1A81-B13D-184D-ACBA-8BA2738F732F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12920" yWindow="2600" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{00C87A90-6B15-DF45-AB5F-3D787AE55E6B}"/>
+    <workbookView xWindow="18600" yWindow="10340" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{00C87A90-6B15-DF45-AB5F-3D787AE55E6B}"/>
   </bookViews>
   <sheets>
     <sheet name="Meta" sheetId="2" r:id="rId1"/>
     <sheet name="COL-Elect-2021-release" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="26">
   <si>
     <t>Electricity</t>
   </si>
@@ -97,13 +97,31 @@
   </si>
   <si>
     <t>COL</t>
+  </si>
+  <si>
+    <t>WRLD</t>
+  </si>
+  <si>
+    <t>2021 Release</t>
+  </si>
+  <si>
+    <t>2022 Release</t>
+  </si>
+  <si>
+    <t>Differences (2022 - 2021)</t>
+  </si>
+  <si>
+    <t>Electricity sum differences (2022 - 2021)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.0000"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -111,8 +129,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -125,6 +158,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -135,14 +173,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -455,35 +501,889 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{784B3D76-9BD3-1A4E-AD29-79E7D5734B47}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:P38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="M33" sqref="M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="10" max="16" width="13.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
     </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="J13">
+        <v>1971</v>
+      </c>
+      <c r="K13">
+        <v>1972</v>
+      </c>
+      <c r="L13">
+        <v>1973</v>
+      </c>
+      <c r="M13">
+        <v>1974</v>
+      </c>
+      <c r="N13">
+        <v>1975</v>
+      </c>
+      <c r="O13">
+        <v>1976</v>
+      </c>
+      <c r="P13">
+        <v>1977</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" t="s">
+        <v>15</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I15" t="s">
+        <v>14</v>
+      </c>
+      <c r="J15" s="1">
+        <v>34196.400800000003</v>
+      </c>
+      <c r="K15" s="1">
+        <v>35456.4015</v>
+      </c>
+      <c r="L15" s="1">
+        <v>39301.198499999999</v>
+      </c>
+      <c r="M15" s="1">
+        <v>44020.7981</v>
+      </c>
+      <c r="N15" s="1">
+        <v>42749.9997</v>
+      </c>
+      <c r="O15" s="1">
+        <v>45496.800000000003</v>
+      </c>
+      <c r="P15" s="1">
+        <v>50983.199500000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" t="s">
+        <v>15</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I16" t="s">
+        <v>14</v>
+      </c>
+      <c r="J16" s="1">
+        <v>2671.1993000000002</v>
+      </c>
+      <c r="K16" s="1">
+        <v>2440.7997</v>
+      </c>
+      <c r="L16" s="1">
+        <v>2555.9994999999999</v>
+      </c>
+      <c r="M16" s="1">
+        <v>2534.3998000000001</v>
+      </c>
+      <c r="N16" s="1">
+        <v>3801.6017999999999</v>
+      </c>
+      <c r="O16" s="1">
+        <v>3844.8011999999999</v>
+      </c>
+      <c r="P16" s="1">
+        <v>3942.002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" t="s">
+        <v>15</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I17" t="s">
+        <v>14</v>
+      </c>
+      <c r="J17" s="5">
+        <v>17919219.890000001</v>
+      </c>
+      <c r="K17" s="5">
+        <v>19448043.870000001</v>
+      </c>
+      <c r="L17" s="5">
+        <v>20927429.399999999</v>
+      </c>
+      <c r="M17" s="5">
+        <v>20188606.5</v>
+      </c>
+      <c r="N17" s="5">
+        <v>21079673.550000001</v>
+      </c>
+      <c r="O17" s="5">
+        <v>22629434.41</v>
+      </c>
+      <c r="P17" s="5">
+        <v>23707132.890000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" t="s">
+        <v>16</v>
+      </c>
+      <c r="F18" t="s">
+        <v>15</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I18" t="s">
+        <v>14</v>
+      </c>
+      <c r="J18" s="5">
+        <v>372117.7096</v>
+      </c>
+      <c r="K18" s="5">
+        <v>376245.55949999997</v>
+      </c>
+      <c r="L18" s="5">
+        <v>401533.76030000002</v>
+      </c>
+      <c r="M18" s="5">
+        <v>1648227.4327</v>
+      </c>
+      <c r="N18" s="5">
+        <v>1569763.0870000001</v>
+      </c>
+      <c r="O18" s="5">
+        <v>1598402.6872</v>
+      </c>
+      <c r="P18" s="5">
+        <v>1649651.602</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
+      <c r="P20" s="3"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" t="s">
+        <v>15</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I21" t="s">
+        <v>14</v>
+      </c>
+      <c r="J21" s="4">
+        <v>31467.599399999999</v>
+      </c>
+      <c r="K21" s="4">
+        <v>32616.001</v>
+      </c>
+      <c r="L21" s="4">
+        <v>36122.399899999997</v>
+      </c>
+      <c r="M21" s="4">
+        <v>40467.599099999999</v>
+      </c>
+      <c r="N21" s="4">
+        <v>40273.201800000003</v>
+      </c>
+      <c r="O21" s="4">
+        <v>42393.598299999998</v>
+      </c>
+      <c r="P21" s="4">
+        <v>47930.398500000003</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22" t="s">
+        <v>16</v>
+      </c>
+      <c r="F22" t="s">
+        <v>15</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I22" t="s">
+        <v>14</v>
+      </c>
+      <c r="J22" s="4">
+        <v>899.99869999999999</v>
+      </c>
+      <c r="K22" s="4">
+        <v>745.2002</v>
+      </c>
+      <c r="L22" s="4">
+        <v>781.19830000000002</v>
+      </c>
+      <c r="M22" s="4">
+        <v>651.6001</v>
+      </c>
+      <c r="N22" s="4">
+        <v>1792.8003000000001</v>
+      </c>
+      <c r="O22" s="4">
+        <v>1695.5996</v>
+      </c>
+      <c r="P22" s="4">
+        <v>1699.2002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" t="s">
+        <v>17</v>
+      </c>
+      <c r="E23" t="s">
+        <v>16</v>
+      </c>
+      <c r="F23" t="s">
+        <v>15</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I23" t="s">
+        <v>14</v>
+      </c>
+      <c r="J23" s="5">
+        <v>17916199.489999998</v>
+      </c>
+      <c r="K23" s="5">
+        <v>19444922.670000002</v>
+      </c>
+      <c r="L23" s="5">
+        <v>20923825.800000001</v>
+      </c>
+      <c r="M23" s="5">
+        <v>20184682.489999998</v>
+      </c>
+      <c r="N23" s="5">
+        <v>21076725.149999999</v>
+      </c>
+      <c r="O23" s="5">
+        <v>22625697.620000001</v>
+      </c>
+      <c r="P23" s="5">
+        <v>23703345.690000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" t="s">
+        <v>17</v>
+      </c>
+      <c r="E24" t="s">
+        <v>16</v>
+      </c>
+      <c r="F24" t="s">
+        <v>15</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I24" t="s">
+        <v>14</v>
+      </c>
+      <c r="J24">
+        <v>369882.1091</v>
+      </c>
+      <c r="K24">
+        <v>374092.76130000001</v>
+      </c>
+      <c r="L24">
+        <v>399236.96130000002</v>
+      </c>
+      <c r="M24">
+        <v>1645779.4316</v>
+      </c>
+      <c r="N24">
+        <v>1567153.0861</v>
+      </c>
+      <c r="O24">
+        <v>1595645.0848999999</v>
+      </c>
+      <c r="P24">
+        <v>1646609.6029000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="3"/>
+      <c r="N26" s="3"/>
+      <c r="O26" s="3"/>
+      <c r="P26" s="3"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>20</v>
+      </c>
+      <c r="B27" t="s">
+        <v>19</v>
+      </c>
+      <c r="C27" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" t="s">
+        <v>17</v>
+      </c>
+      <c r="E27" t="s">
+        <v>16</v>
+      </c>
+      <c r="F27" t="s">
+        <v>15</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I27" t="s">
+        <v>14</v>
+      </c>
+      <c r="J27">
+        <f>J21-J15</f>
+        <v>-2728.8014000000039</v>
+      </c>
+      <c r="K27">
+        <f t="shared" ref="K27:P27" si="0">K21-K15</f>
+        <v>-2840.4004999999997</v>
+      </c>
+      <c r="L27">
+        <f t="shared" si="0"/>
+        <v>-3178.7986000000019</v>
+      </c>
+      <c r="M27">
+        <f t="shared" si="0"/>
+        <v>-3553.1990000000005</v>
+      </c>
+      <c r="N27">
+        <f t="shared" si="0"/>
+        <v>-2476.7978999999978</v>
+      </c>
+      <c r="O27">
+        <f t="shared" si="0"/>
+        <v>-3103.2017000000051</v>
+      </c>
+      <c r="P27">
+        <f t="shared" si="0"/>
+        <v>-3052.8009999999995</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" t="s">
+        <v>19</v>
+      </c>
+      <c r="C28" t="s">
+        <v>18</v>
+      </c>
+      <c r="D28" t="s">
+        <v>17</v>
+      </c>
+      <c r="E28" t="s">
+        <v>16</v>
+      </c>
+      <c r="F28" t="s">
+        <v>15</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I28" t="s">
+        <v>14</v>
+      </c>
+      <c r="J28">
+        <f t="shared" ref="J28:P28" si="1">J22-J16</f>
+        <v>-1771.2006000000001</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="1"/>
+        <v>-1695.5995</v>
+      </c>
+      <c r="L28">
+        <f t="shared" si="1"/>
+        <v>-1774.8011999999999</v>
+      </c>
+      <c r="M28">
+        <f t="shared" si="1"/>
+        <v>-1882.7997</v>
+      </c>
+      <c r="N28">
+        <f t="shared" si="1"/>
+        <v>-2008.8014999999998</v>
+      </c>
+      <c r="O28">
+        <f t="shared" si="1"/>
+        <v>-2149.2015999999999</v>
+      </c>
+      <c r="P28">
+        <f t="shared" si="1"/>
+        <v>-2242.8018000000002</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>21</v>
+      </c>
+      <c r="B29" t="s">
+        <v>19</v>
+      </c>
+      <c r="C29" t="s">
+        <v>18</v>
+      </c>
+      <c r="D29" t="s">
+        <v>17</v>
+      </c>
+      <c r="E29" t="s">
+        <v>16</v>
+      </c>
+      <c r="F29" t="s">
+        <v>15</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I29" t="s">
+        <v>14</v>
+      </c>
+      <c r="J29">
+        <f t="shared" ref="J29:P29" si="2">J23-J17</f>
+        <v>-3020.4000000022352</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="2"/>
+        <v>-3121.1999999992549</v>
+      </c>
+      <c r="L29">
+        <f t="shared" si="2"/>
+        <v>-3603.5999999977648</v>
+      </c>
+      <c r="M29">
+        <f t="shared" si="2"/>
+        <v>-3924.0100000016391</v>
+      </c>
+      <c r="N29">
+        <f t="shared" si="2"/>
+        <v>-2948.4000000022352</v>
+      </c>
+      <c r="O29">
+        <f t="shared" si="2"/>
+        <v>-3736.7899999991059</v>
+      </c>
+      <c r="P29">
+        <f t="shared" si="2"/>
+        <v>-3787.1999999992549</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>21</v>
+      </c>
+      <c r="B30" t="s">
+        <v>19</v>
+      </c>
+      <c r="C30" t="s">
+        <v>18</v>
+      </c>
+      <c r="D30" t="s">
+        <v>17</v>
+      </c>
+      <c r="E30" t="s">
+        <v>16</v>
+      </c>
+      <c r="F30" t="s">
+        <v>15</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I30" t="s">
+        <v>14</v>
+      </c>
+      <c r="J30">
+        <f t="shared" ref="J30:P30" si="3">J24-J18</f>
+        <v>-2235.6005000000005</v>
+      </c>
+      <c r="K30">
+        <f t="shared" si="3"/>
+        <v>-2152.7981999999611</v>
+      </c>
+      <c r="L30">
+        <f t="shared" si="3"/>
+        <v>-2296.7989999999991</v>
+      </c>
+      <c r="M30">
+        <f t="shared" si="3"/>
+        <v>-2448.001099999994</v>
+      </c>
+      <c r="N30">
+        <f t="shared" si="3"/>
+        <v>-2610.000900000101</v>
+      </c>
+      <c r="O30">
+        <f t="shared" si="3"/>
+        <v>-2757.6023000001442</v>
+      </c>
+      <c r="P30">
+        <f t="shared" si="3"/>
+        <v>-3041.999099999899</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3"/>
+      <c r="M32" s="3"/>
+      <c r="N32" s="3"/>
+      <c r="O32" s="3"/>
+      <c r="P32" s="3"/>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>20</v>
+      </c>
+      <c r="B33" t="s">
+        <v>19</v>
+      </c>
+      <c r="C33" t="s">
+        <v>18</v>
+      </c>
+      <c r="D33" t="s">
+        <v>17</v>
+      </c>
+      <c r="E33" t="s">
+        <v>16</v>
+      </c>
+      <c r="F33" t="s">
+        <v>15</v>
+      </c>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I33" t="s">
+        <v>14</v>
+      </c>
+      <c r="J33">
+        <f>SUM(J27:J28)</f>
+        <v>-4500.002000000004</v>
+      </c>
+      <c r="K33">
+        <f t="shared" ref="K33:P33" si="4">SUM(K27:K28)</f>
+        <v>-4536</v>
+      </c>
+      <c r="L33">
+        <f t="shared" si="4"/>
+        <v>-4953.5998000000018</v>
+      </c>
+      <c r="M33">
+        <f t="shared" si="4"/>
+        <v>-5435.9987000000001</v>
+      </c>
+      <c r="N33">
+        <f t="shared" si="4"/>
+        <v>-4485.5993999999973</v>
+      </c>
+      <c r="O33">
+        <f t="shared" si="4"/>
+        <v>-5252.4033000000054</v>
+      </c>
+      <c r="P33">
+        <f t="shared" si="4"/>
+        <v>-5295.6027999999997</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>21</v>
+      </c>
+      <c r="B34" t="s">
+        <v>19</v>
+      </c>
+      <c r="C34" t="s">
+        <v>18</v>
+      </c>
+      <c r="D34" t="s">
+        <v>17</v>
+      </c>
+      <c r="E34" t="s">
+        <v>16</v>
+      </c>
+      <c r="F34" t="s">
+        <v>15</v>
+      </c>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I34" t="s">
+        <v>14</v>
+      </c>
+      <c r="J34">
+        <f>SUM(J29:J30)</f>
+        <v>-5256.0005000022356</v>
+      </c>
+      <c r="K34">
+        <f t="shared" ref="K34:P34" si="5">SUM(K29:K30)</f>
+        <v>-5273.998199999216</v>
+      </c>
+      <c r="L34">
+        <f t="shared" si="5"/>
+        <v>-5900.3989999977639</v>
+      </c>
+      <c r="M34">
+        <f t="shared" si="5"/>
+        <v>-6372.0111000016332</v>
+      </c>
+      <c r="N34">
+        <f t="shared" si="5"/>
+        <v>-5558.4009000023361</v>
+      </c>
+      <c r="O34">
+        <f t="shared" si="5"/>
+        <v>-6494.3922999992501</v>
+      </c>
+      <c r="P34">
+        <f t="shared" si="5"/>
+        <v>-6829.199099999154</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="J38" s="5"/>
+    </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A14:P14"/>
+    <mergeCell ref="A20:P20"/>
+    <mergeCell ref="A26:P26"/>
+    <mergeCell ref="A32:P32"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B48302AA-2E8E-234B-A5A4-DF82F724CD82}">
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="J1" sqref="J1:P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -641,6 +1541,106 @@
         <v>3942.002</v>
       </c>
     </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" s="2">
+        <v>17919219.890000001</v>
+      </c>
+      <c r="K4" s="2">
+        <v>19448043.870000001</v>
+      </c>
+      <c r="L4" s="2">
+        <v>20927429.399999999</v>
+      </c>
+      <c r="M4" s="2">
+        <v>20188606.5</v>
+      </c>
+      <c r="N4" s="2">
+        <v>21079673.550000001</v>
+      </c>
+      <c r="O4" s="2">
+        <v>22629434.41</v>
+      </c>
+      <c r="P4" s="2">
+        <v>23707132.890000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5">
+        <v>372117.7096</v>
+      </c>
+      <c r="K5">
+        <v>376245.55949999997</v>
+      </c>
+      <c r="L5">
+        <v>401533.76030000002</v>
+      </c>
+      <c r="M5">
+        <v>1648227.4327</v>
+      </c>
+      <c r="N5">
+        <v>1569763.0870000001</v>
+      </c>
+      <c r="O5">
+        <v>1598402.6872</v>
+      </c>
+      <c r="P5">
+        <v>1649651.602</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>